<commit_message>
Fix bug in ExcelService
</commit_message>
<xml_diff>
--- a/exporter/src/main/resources/templates/rp-template.xlsx
+++ b/exporter/src/main/resources/templates/rp-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\code\Spring_Boot\Excel_Export_Spring\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\SpringProject\Excel_Export_Sping_Boot-main\exporter\src\main\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ABC5D03-C2E6-4421-B221-37031D8423B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42CD0D81-A059-458B-8908-55A09B6D2BE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B1CB01FB-7046-4E23-ADE0-655E702C4B34}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B1CB01FB-7046-4E23-ADE0-655E702C4B34}"/>
   </bookViews>
   <sheets>
     <sheet name="BC" sheetId="2" r:id="rId1"/>
@@ -265,7 +265,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -288,14 +288,6 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -317,8 +309,11 @@
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -328,12 +323,6 @@
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -649,104 +638,104 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8753B0FC-8F86-410C-8F46-FAB7A5657CB4}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="37.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="51.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="18.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="47.42578125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="27.85546875" style="3" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="9.109375" style="1"/>
+    <col min="2" max="2" width="37.6640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="51.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="18.6640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="47.44140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="27.88671875" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.15">
-      <c r="B2" s="10" t="s">
+    <row r="1" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="11"/>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B3" s="12" t="s">
+      <c r="C2" s="9"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="13"/>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B4" s="12" t="s">
+      <c r="C3" s="11"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="13"/>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B5" s="12" t="s">
+      <c r="C4" s="11"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="13"/>
-    </row>
-    <row r="6" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="14" t="s">
+      <c r="C5" s="11"/>
+    </row>
+    <row r="6" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="15"/>
-    </row>
-    <row r="7" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C6" s="13"/>
+    </row>
+    <row r="7" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="G9" s="20"/>
-    </row>
-    <row r="10" spans="2:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="17" t="s">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G9" s="14"/>
+    </row>
+    <row r="10" spans="2:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B10" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="21" t="s">
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="18" t="s">
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B12" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="19" t="s">
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D14" s="5"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B15" s="6" t="s">
         <v>1</v>
       </c>
@@ -765,25 +754,6 @@
       <c r="G15" s="7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="6"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="8"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="6"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="8"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>